<commit_message>
30 Apr 2024 - Candidates can now jump directly to any question during the test.
</commit_message>
<xml_diff>
--- a/static/scores/VM_1113_scores.xlsx
+++ b/static/scores/VM_1113_scores.xlsx
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -534,7 +534,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>